<commit_message>
creating figures for poster
</commit_message>
<xml_diff>
--- a/data/raw/eSTZ_consistency_formatting.xlsx
+++ b/data/raw/eSTZ_consistency_formatting.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Raw File Paths" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2495" uniqueCount="576">
   <si>
     <t xml:space="preserve">File 1 -&gt;</t>
   </si>
@@ -2482,6 +2482,9 @@
   </si>
   <si>
     <t xml:space="preserve">Note: Total should be 20 (does not include 5 with no map or provisional seed zones maps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MapFeature-Ecotype_Description</t>
   </si>
   <si>
     <t xml:space="preserve">MapFeature-Ploidy_Key</t>
@@ -3162,11 +3165,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="94458788"/>
-        <c:axId val="7190176"/>
+        <c:axId val="33258401"/>
+        <c:axId val="10456273"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94458788"/>
+        <c:axId val="33258401"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3199,7 +3202,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7190176"/>
+        <c:crossAx val="10456273"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3207,7 +3210,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7190176"/>
+        <c:axId val="10456273"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3247,7 +3250,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94458788"/>
+        <c:crossAx val="33258401"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3389,11 +3392,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="14929163"/>
-        <c:axId val="3103334"/>
+        <c:axId val="86535561"/>
+        <c:axId val="1226554"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="14929163"/>
+        <c:axId val="86535561"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3426,7 +3429,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3103334"/>
+        <c:crossAx val="1226554"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3434,7 +3437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3103334"/>
+        <c:axId val="1226554"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3474,7 +3477,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14929163"/>
+        <c:crossAx val="86535561"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3694,11 +3697,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="36331128"/>
-        <c:axId val="98572391"/>
+        <c:axId val="17501551"/>
+        <c:axId val="44126038"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="36331128"/>
+        <c:axId val="17501551"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3731,7 +3734,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98572391"/>
+        <c:crossAx val="44126038"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3739,7 +3742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98572391"/>
+        <c:axId val="44126038"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3779,7 +3782,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36331128"/>
+        <c:crossAx val="17501551"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3895,10 +3898,10 @@
                   <c:v>MapFeature-Zone_Key</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>MapFeature-Ecotype_Discription</c:v>
+                  <c:v>MapFeature-Ecotype_Description</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>MapFeature-Ecotype_Discription</c:v>
+                  <c:v>MapFeature-Ecotype_Description</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>MapFeature-Percent_Cover</c:v>
@@ -4107,11 +4110,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="43361421"/>
-        <c:axId val="46221327"/>
+        <c:axId val="1234722"/>
+        <c:axId val="71920498"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43361421"/>
+        <c:axId val="1234722"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4144,7 +4147,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46221327"/>
+        <c:crossAx val="71920498"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4152,7 +4155,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46221327"/>
+        <c:axId val="71920498"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4192,7 +4195,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43361421"/>
+        <c:crossAx val="1234722"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4358,11 +4361,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="34155056"/>
-        <c:axId val="95706713"/>
+        <c:axId val="78629627"/>
+        <c:axId val="9473481"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="34155056"/>
+        <c:axId val="78629627"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4395,7 +4398,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95706713"/>
+        <c:crossAx val="9473481"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4403,7 +4406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95706713"/>
+        <c:axId val="9473481"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4443,7 +4446,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34155056"/>
+        <c:crossAx val="78629627"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4482,9 +4485,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>816480</xdr:colOff>
+      <xdr:colOff>816120</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>97560</xdr:rowOff>
+      <xdr:rowOff>97200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4492,8 +4495,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5558400" y="2060280"/>
-        <a:ext cx="5839560" cy="4838040"/>
+        <a:off x="5559840" y="2060280"/>
+        <a:ext cx="5845680" cy="4837680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4517,9 +4520,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
+      <xdr:colOff>65520</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>27360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4527,8 +4530,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3021840" y="1600200"/>
-        <a:ext cx="5839920" cy="4828320"/>
+        <a:off x="3024360" y="1600200"/>
+        <a:ext cx="5846040" cy="4827960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4552,9 +4555,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>309240</xdr:colOff>
+      <xdr:colOff>308880</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4562,8 +4565,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8340840" y="2327400"/>
-        <a:ext cx="4244760" cy="2882160"/>
+        <a:off x="8346960" y="2327400"/>
+        <a:ext cx="4248360" cy="2881800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4587,9 +4590,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>21240</xdr:rowOff>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4597,8 +4600,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4662720" y="1082520"/>
-        <a:ext cx="7187400" cy="5939640"/>
+        <a:off x="4666320" y="1082520"/>
+        <a:ext cx="7197480" cy="5939280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4622,9 +4625,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>662760</xdr:colOff>
+      <xdr:colOff>662400</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4632,8 +4635,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6365880" y="2933640"/>
-        <a:ext cx="4257360" cy="2882160"/>
+        <a:off x="6374880" y="2933640"/>
+        <a:ext cx="4262040" cy="2881800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4653,13 +4656,13 @@
   </sheetPr>
   <dimension ref="A1:Z297"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="E174" activeCellId="0" sqref="E174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.66"/>
@@ -15728,7 +15731,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.33"/>
@@ -15809,7 +15812,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.66"/>
@@ -16027,7 +16030,7 @@
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.67"/>
@@ -16126,7 +16129,7 @@
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.52"/>
@@ -16478,7 +16481,7 @@
       <selection pane="bottomLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.16"/>
@@ -19025,11 +19028,11 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.66"/>
   </cols>
@@ -19113,7 +19116,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>528</v>
+        <v>547</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>1</v>
@@ -19124,7 +19127,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>528</v>
+        <v>547</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>19</v>
@@ -19157,7 +19160,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>1</v>
@@ -19168,7 +19171,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>19</v>
@@ -19399,7 +19402,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="22" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B34" s="3" t="n">
         <v>11</v>
@@ -19410,7 +19413,7 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="B35" s="3" t="n">
         <v>9</v>
@@ -19467,7 +19470,7 @@
       <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.16"/>
@@ -19482,7 +19485,7 @@
         <v>426</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -19518,7 +19521,7 @@
         <v>448</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19529,7 +19532,7 @@
         <v>457</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19540,7 +19543,7 @@
         <v>459</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19551,7 +19554,7 @@
         <v>460</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19562,7 +19565,7 @@
         <v>461</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19573,7 +19576,7 @@
         <v>463</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19584,7 +19587,7 @@
         <v>467</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19595,7 +19598,7 @@
         <v>471</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19606,7 +19609,7 @@
         <v>475</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19617,7 +19620,7 @@
         <v>477</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19628,7 +19631,7 @@
         <v>479</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19639,7 +19642,7 @@
         <v>481</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19650,7 +19653,7 @@
         <v>483</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19661,7 +19664,7 @@
         <v>492</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19672,7 +19675,7 @@
         <v>498</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19683,7 +19686,7 @@
         <v>500</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19694,7 +19697,7 @@
         <v>502</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19705,7 +19708,7 @@
         <v>503</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19716,7 +19719,7 @@
         <v>508</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19727,7 +19730,7 @@
         <v>509</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19738,7 +19741,7 @@
         <v>510</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19749,7 +19752,7 @@
         <v>486</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19760,7 +19763,7 @@
         <v>489</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19793,7 +19796,7 @@
         <v>512</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19815,7 +19818,7 @@
         <v>515</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19826,7 +19829,7 @@
         <v>521</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -19845,32 +19848,32 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B36" s="3" t="n">
         <v>21</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B37" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B38" s="3" t="n">
         <v>2</v>
@@ -19881,12 +19884,12 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="3" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -19911,7 +19914,7 @@
       <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.84765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -19926,29 +19929,29 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>2</v>

</xml_diff>